<commit_message>
Tetris v.0.11.1 / VGA docs
</commit_message>
<xml_diff>
--- a/2nd gen - 8 bit cpu/VGA output/VGA timings with 5MHz pixel clock.xlsx
+++ b/2nd gen - 8 bit cpu/VGA output/VGA timings with 5MHz pixel clock.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="23955" windowHeight="11310"/>
+    <workbookView xWindow="360" yWindow="165" windowWidth="23955" windowHeight="11250"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>Source:</t>
   </si>
@@ -66,13 +66,19 @@
     <t>5 MHz</t>
   </si>
   <si>
-    <t>same</t>
-  </si>
-  <si>
     <t>Resolution: 128 x 96</t>
   </si>
   <si>
     <t>5 lines repeated (480 / 5 = 96)</t>
+  </si>
+  <si>
+    <t>Lines</t>
+  </si>
+  <si>
+    <t>Bytes used (1 byte/pixel)</t>
+  </si>
+  <si>
+    <t>1 MHz</t>
   </si>
 </sst>
 </file>
@@ -152,13 +158,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -461,38 +472,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4"/>
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5"/>
+      <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="E1" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -507,8 +523,12 @@
         <f>C3/2</f>
         <v>128</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="3">
+        <f>B3/20</f>
+        <v>25.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -516,15 +536,19 @@
         <v>12</v>
       </c>
       <c r="C4" s="3">
-        <f t="shared" ref="C4:D7" si="0">B4/2</f>
+        <f t="shared" ref="C4:E7" si="0">B4/2</f>
         <v>6</v>
       </c>
       <c r="D4" s="3">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="3">
+        <f t="shared" ref="E4:E7" si="1">B4/20</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -539,8 +563,12 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="3">
+        <f t="shared" si="1"/>
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -555,8 +583,12 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="3">
+        <f t="shared" si="1"/>
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
@@ -572,36 +604,45 @@
         <f t="shared" si="0"/>
         <v>159</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="3">
+        <f t="shared" si="1"/>
+        <v>31.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
-    </row>
-    <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="3">
         <v>480</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10" s="3">
+        <v>480</v>
+      </c>
+      <c r="D10" s="3">
+        <v>480</v>
+      </c>
+      <c r="E10" s="3">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
@@ -610,8 +651,9 @@
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
@@ -620,8 +662,9 @@
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
@@ -630,8 +673,9 @@
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>8</v>
       </c>
@@ -641,28 +685,71 @@
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D16" t="s">
+      <c r="E14" s="3"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16">
+        <f>B10</f>
+        <v>480</v>
+      </c>
+      <c r="C16">
+        <f>C10/2</f>
+        <v>240</v>
+      </c>
+      <c r="D16">
+        <f>$D10/4</f>
+        <v>120</v>
+      </c>
+      <c r="E16">
+        <f>$D10/5</f>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17">
+        <f>B3*B16</f>
+        <v>245760</v>
+      </c>
+      <c r="C17">
+        <f>C3*C16</f>
+        <v>61440</v>
+      </c>
+      <c r="D17">
+        <f>$D3*D16</f>
+        <v>15360</v>
+      </c>
+      <c r="E17">
+        <f>$D3*E16</f>
+        <v>12288</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
         <v>0</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C28" r:id="rId1"/>
+    <hyperlink ref="C32" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
Changes in docs/reorganizing files
</commit_message>
<xml_diff>
--- a/2nd gen - 8 bit cpu/VGA output/VGA timings with 5MHz pixel clock.xlsx
+++ b/2nd gen - 8 bit cpu/VGA output/VGA timings with 5MHz pixel clock.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\albs_\Source\Repos\jaca\2nd gen - 8 bit cpu\VGA output\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{98FA2ADE-0FAE-4459-B60F-E686AC50D743}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="165" windowWidth="23955" windowHeight="11250"/>
+    <workbookView xWindow="360" yWindow="168" windowWidth="23952" windowHeight="11256" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
     <sheet name="Plan2" sheetId="2" r:id="rId2"/>
     <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Source:</t>
   </si>
@@ -30,36 +36,12 @@
     <t>Horiz</t>
   </si>
   <si>
-    <t>HPX</t>
-  </si>
-  <si>
-    <t>HFP</t>
-  </si>
-  <si>
-    <t>HSP</t>
-  </si>
-  <si>
-    <t>HBP</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
     <t>Vert</t>
   </si>
   <si>
-    <t>VLN</t>
-  </si>
-  <si>
-    <t>VFP</t>
-  </si>
-  <si>
-    <t>VSP</t>
-  </si>
-  <si>
-    <t>VBP</t>
-  </si>
-  <si>
     <t>10 MHz</t>
   </si>
   <si>
@@ -79,12 +61,45 @@
   </si>
   <si>
     <t>1 MHz</t>
+  </si>
+  <si>
+    <t>Other tries (only 2 and 4 leads to integer results):</t>
+  </si>
+  <si>
+    <t>HPX (Horiz. Pixels)</t>
+  </si>
+  <si>
+    <t>HFP (Horiz. Front Porch)</t>
+  </si>
+  <si>
+    <t>HSP (Horiz. Sync Pulse)</t>
+  </si>
+  <si>
+    <t>HBP (Horiz. Back Porch)</t>
+  </si>
+  <si>
+    <t>VLN (Vert. Lines)</t>
+  </si>
+  <si>
+    <t>VFP (Vert. Front Porch)</t>
+  </si>
+  <si>
+    <t>VSP (Vert. Sync Pulse)</t>
+  </si>
+  <si>
+    <t>VBP (Vert. Back Porch)</t>
+  </si>
+  <si>
+    <t>Time (sec.)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.0000000000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -130,7 +145,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -153,12 +168,128 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -170,9 +301,41 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -181,14 +344,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -226,9 +392,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -261,9 +427,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -296,9 +479,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -471,225 +671,703 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Z32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5"/>
       <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="15"/>
+      <c r="F1" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C2" s="9"/>
+      <c r="D2" s="25">
+        <f>1/5000000</f>
+        <v>1.9999999999999999E-7</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="12"/>
+      <c r="H2" s="2">
+        <v>2</v>
+      </c>
+      <c r="I2" s="2">
+        <v>3</v>
+      </c>
+      <c r="J2" s="2">
+        <v>4</v>
+      </c>
+      <c r="K2" s="2">
+        <v>5</v>
+      </c>
+      <c r="L2" s="2">
+        <v>6</v>
+      </c>
+      <c r="M2" s="2">
+        <v>7</v>
+      </c>
+      <c r="N2" s="2">
+        <v>8</v>
+      </c>
+      <c r="O2" s="2">
+        <v>9</v>
+      </c>
+      <c r="P2" s="2">
+        <v>10</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>11</v>
+      </c>
+      <c r="R2" s="2">
+        <v>12</v>
+      </c>
+      <c r="S2" s="2">
+        <v>13</v>
+      </c>
+      <c r="T2" s="2">
+        <v>14</v>
+      </c>
+      <c r="U2" s="2">
+        <v>15</v>
+      </c>
+      <c r="V2" s="2">
+        <v>16</v>
+      </c>
+      <c r="W2" s="2">
+        <v>17</v>
+      </c>
+      <c r="X2" s="2">
+        <v>18</v>
+      </c>
+      <c r="Y2" s="2">
+        <v>19</v>
+      </c>
+      <c r="Z2" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B3" s="3">
         <v>512</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="10">
         <f>B3/2</f>
         <v>256</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="18">
         <f>C3/2</f>
         <v>128</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="26">
+        <f>D3*$D$2</f>
+        <v>2.5599999999999999E-5</v>
+      </c>
+      <c r="F3" s="13">
         <f>B3/20</f>
         <v>25.6</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <f>$B3/H$2</f>
+        <v>256</v>
+      </c>
+      <c r="I3">
+        <f>$B3/I$2</f>
+        <v>170.66666666666666</v>
+      </c>
+      <c r="J3">
+        <f>$B3/J$2</f>
+        <v>128</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:Z7" si="0">$B3/K$2</f>
+        <v>102.4</v>
+      </c>
+      <c r="L3">
+        <f t="shared" si="0"/>
+        <v>85.333333333333329</v>
+      </c>
+      <c r="M3">
+        <f t="shared" si="0"/>
+        <v>73.142857142857139</v>
+      </c>
+      <c r="N3">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="O3">
+        <f t="shared" si="0"/>
+        <v>56.888888888888886</v>
+      </c>
+      <c r="P3">
+        <f t="shared" si="0"/>
+        <v>51.2</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" si="0"/>
+        <v>46.545454545454547</v>
+      </c>
+      <c r="R3">
+        <f t="shared" si="0"/>
+        <v>42.666666666666664</v>
+      </c>
+      <c r="S3">
+        <f t="shared" si="0"/>
+        <v>39.384615384615387</v>
+      </c>
+      <c r="T3">
+        <f t="shared" si="0"/>
+        <v>36.571428571428569</v>
+      </c>
+      <c r="U3">
+        <f t="shared" si="0"/>
+        <v>34.133333333333333</v>
+      </c>
+      <c r="V3">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="W3">
+        <f t="shared" si="0"/>
+        <v>30.117647058823529</v>
+      </c>
+      <c r="X3">
+        <f t="shared" si="0"/>
+        <v>28.444444444444443</v>
+      </c>
+      <c r="Y3">
+        <f t="shared" si="0"/>
+        <v>26.94736842105263</v>
+      </c>
+      <c r="Z3">
+        <f t="shared" si="0"/>
+        <v>25.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B4" s="3">
         <v>12</v>
       </c>
-      <c r="C4" s="3">
-        <f t="shared" ref="C4:D7" si="0">B4/2</f>
+      <c r="C4" s="10">
+        <f t="shared" ref="C4:D7" si="1">B4/2</f>
         <v>6</v>
       </c>
-      <c r="D4" s="3">
-        <f t="shared" si="0"/>
+      <c r="D4" s="18">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="E4" s="3">
-        <f t="shared" ref="E4:E7" si="1">B4/20</f>
+      <c r="E4" s="19">
+        <f>D4*$D$2</f>
+        <v>5.9999999999999997E-7</v>
+      </c>
+      <c r="F4" s="13">
+        <f t="shared" ref="F4:F7" si="2">B4/20</f>
         <v>0.6</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H4">
+        <f t="shared" ref="H4:W7" si="3">$B4/H$2</f>
+        <v>6</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="3"/>
+        <v>2.4</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="3"/>
+        <v>1.7142857142857142</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="3"/>
+        <v>1.5</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="3"/>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="3"/>
+        <v>1.2</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="3"/>
+        <v>1.0909090909090908</v>
+      </c>
+      <c r="R4">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="S4">
+        <f t="shared" si="3"/>
+        <v>0.92307692307692313</v>
+      </c>
+      <c r="T4">
+        <f t="shared" si="3"/>
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="U4">
+        <f t="shared" si="3"/>
+        <v>0.8</v>
+      </c>
+      <c r="V4">
+        <f t="shared" si="3"/>
+        <v>0.75</v>
+      </c>
+      <c r="W4">
+        <f t="shared" si="3"/>
+        <v>0.70588235294117652</v>
+      </c>
+      <c r="X4">
+        <f t="shared" si="0"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="Y4">
+        <f t="shared" si="0"/>
+        <v>0.63157894736842102</v>
+      </c>
+      <c r="Z4">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B5" s="3">
         <v>76</v>
       </c>
-      <c r="C5" s="3">
-        <f t="shared" si="0"/>
+      <c r="C5" s="10">
+        <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="D5" s="3">
-        <f t="shared" si="0"/>
+      <c r="D5" s="18">
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="E5" s="3">
-        <f t="shared" si="1"/>
+      <c r="E5" s="19">
+        <f>D5*$D$2</f>
+        <v>3.8E-6</v>
+      </c>
+      <c r="F5" s="13">
+        <f t="shared" si="2"/>
         <v>3.8</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H5">
+        <f t="shared" si="3"/>
+        <v>38</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="3"/>
+        <v>25.333333333333332</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>15.2</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>12.666666666666666</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="0"/>
+        <v>10.857142857142858</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="0"/>
+        <v>9.5</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="0"/>
+        <v>8.4444444444444446</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="0"/>
+        <v>7.6</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="0"/>
+        <v>6.9090909090909092</v>
+      </c>
+      <c r="R5">
+        <f t="shared" si="0"/>
+        <v>6.333333333333333</v>
+      </c>
+      <c r="S5">
+        <f t="shared" si="0"/>
+        <v>5.8461538461538458</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="0"/>
+        <v>5.4285714285714288</v>
+      </c>
+      <c r="U5">
+        <f t="shared" si="0"/>
+        <v>5.0666666666666664</v>
+      </c>
+      <c r="V5">
+        <f t="shared" si="0"/>
+        <v>4.75</v>
+      </c>
+      <c r="W5">
+        <f t="shared" si="0"/>
+        <v>4.4705882352941178</v>
+      </c>
+      <c r="X5">
+        <f t="shared" si="0"/>
+        <v>4.2222222222222223</v>
+      </c>
+      <c r="Y5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="Z5">
+        <f t="shared" si="0"/>
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B6" s="3">
         <v>36</v>
       </c>
-      <c r="C6" s="3">
-        <f t="shared" si="0"/>
+      <c r="C6" s="10">
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="D6" s="3">
-        <f t="shared" si="0"/>
+      <c r="D6" s="18">
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="E6" s="3">
-        <f t="shared" si="1"/>
+      <c r="E6" s="19">
+        <f>D6*$D$2</f>
+        <v>1.7999999999999999E-6</v>
+      </c>
+      <c r="F6" s="13">
+        <f t="shared" si="2"/>
         <v>1.8</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H6">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>7.2</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="0"/>
+        <v>5.1428571428571432</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="0"/>
+        <v>4.5</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="0"/>
+        <v>3.6</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="0"/>
+        <v>3.2727272727272729</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="S6">
+        <f t="shared" si="0"/>
+        <v>2.7692307692307692</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="0"/>
+        <v>2.5714285714285716</v>
+      </c>
+      <c r="U6">
+        <f t="shared" si="0"/>
+        <v>2.4</v>
+      </c>
+      <c r="V6">
+        <f t="shared" si="0"/>
+        <v>2.25</v>
+      </c>
+      <c r="W6">
+        <f t="shared" si="0"/>
+        <v>2.1176470588235294</v>
+      </c>
+      <c r="X6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="Y6">
+        <f t="shared" si="0"/>
+        <v>1.8947368421052631</v>
+      </c>
+      <c r="Z6">
+        <f t="shared" si="0"/>
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B7" s="3">
         <f>SUM(B3:B6)</f>
         <v>636</v>
       </c>
-      <c r="C7" s="3">
-        <f t="shared" si="0"/>
+      <c r="C7" s="10">
+        <f t="shared" si="1"/>
         <v>318</v>
       </c>
-      <c r="D7" s="3">
-        <f t="shared" si="0"/>
+      <c r="D7" s="18">
+        <f t="shared" si="1"/>
         <v>159</v>
       </c>
-      <c r="E7" s="3">
-        <f t="shared" si="1"/>
+      <c r="E7" s="19">
+        <f>D7*$D$2</f>
+        <v>3.18E-5</v>
+      </c>
+      <c r="F7" s="13">
+        <f t="shared" si="2"/>
         <v>31.8</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H7">
+        <f t="shared" si="3"/>
+        <v>318</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="3"/>
+        <v>212</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="3"/>
+        <v>159</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="0"/>
+        <v>127.2</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>106</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="0"/>
+        <v>90.857142857142861</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="0"/>
+        <v>79.5</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="0"/>
+        <v>70.666666666666671</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="0"/>
+        <v>63.6</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="0"/>
+        <v>57.81818181818182</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="0"/>
+        <v>48.92307692307692</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="0"/>
+        <v>45.428571428571431</v>
+      </c>
+      <c r="U7">
+        <f t="shared" si="0"/>
+        <v>42.4</v>
+      </c>
+      <c r="V7">
+        <f t="shared" si="0"/>
+        <v>39.75</v>
+      </c>
+      <c r="W7">
+        <f t="shared" si="0"/>
+        <v>37.411764705882355</v>
+      </c>
+      <c r="X7">
+        <f t="shared" si="0"/>
+        <v>35.333333333333336</v>
+      </c>
+      <c r="Y7">
+        <f t="shared" si="0"/>
+        <v>33.473684210526315</v>
+      </c>
+      <c r="Z7">
+        <f t="shared" si="0"/>
+        <v>31.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="10"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="13"/>
+    </row>
+    <row r="9" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C9" s="9"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="12"/>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B10" s="3">
         <v>480</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="10">
         <v>480</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="18">
         <v>480</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="20"/>
+      <c r="F10" s="13">
         <v>480</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B11" s="3">
         <v>11</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C11" s="10"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="13"/>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B12" s="3">
         <v>2</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C12" s="10"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="13"/>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B13" s="3">
         <v>31</v>
       </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>8</v>
+      <c r="C13" s="10"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="13"/>
+    </row>
+    <row r="14" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="23" t="s">
+        <v>4</v>
       </c>
       <c r="B14" s="3">
         <f>SUM(B10:B13)</f>
         <v>524</v>
       </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C14" s="10"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="13"/>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B16">
         <f>B10</f>
@@ -703,14 +1381,14 @@
         <f>$D10/5</f>
         <v>96</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <f>$D10/5</f>
         <v>96</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B17">
         <f>B3*B16</f>
@@ -724,22 +1402,22 @@
         <f>$D3*D16</f>
         <v>12288</v>
       </c>
-      <c r="E17">
-        <f>$D3*E16</f>
+      <c r="F17">
+        <f>$D3*F16</f>
         <v>12288</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D21" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>0</v>
       </c>
@@ -749,7 +1427,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C32" r:id="rId1"/>
+    <hyperlink ref="C32" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -757,24 +1435,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>